<commit_message>
commonfields introduced WIP on db access dataTypes.xlsx name changed to application.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/fm/spec/form/form2.xlsx
+++ b/src/main/resources/fm/spec/form/form2.xlsx
@@ -29,13 +29,13 @@
     <t>Sl No</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
   <si>
     <t>True/False</t>
@@ -44,13 +44,13 @@
     <t>Description</t>
   </si>
   <si>
+    <t>references to otherdocuments ofrelevance to this form</t>
+  </si>
+  <si>
     <t>userIdFieldName</t>
   </si>
   <si>
     <t>All notes,including Q&amp;A about this form</t>
-  </si>
-  <si>
-    <t>references to otherdocuments ofrelevance to this form</t>
   </si>
   <si>
     <t>getAllowed</t>
@@ -101,6 +101,9 @@
     <t>Field Name</t>
   </si>
   <si>
+    <t>tableName</t>
+  </si>
+  <si>
     <t>Label</t>
   </si>
   <si>
@@ -131,15 +134,6 @@
     <t>value List Name</t>
   </si>
   <si>
-    <t>tableName</t>
-  </si>
-  <si>
-    <t>Value List Key Field</t>
-  </si>
-  <si>
-    <t>productId</t>
-  </si>
-  <si>
     <t>Form Name</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>Max Rows</t>
+  </si>
+  <si>
+    <t>Value List Key Field</t>
+  </si>
+  <si>
+    <t>productId</t>
   </si>
   <si>
     <t>Product Id</t>
@@ -353,7 +353,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -376,7 +376,7 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -5782,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -5805,7 +5805,7 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -11209,7 +11209,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -11236,7 +11236,7 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -19824,6 +19824,7 @@
     <col customWidth="1" min="9" max="9" width="9.86"/>
     <col customWidth="1" min="10" max="10" width="9.14"/>
     <col customWidth="1" min="11" max="11" width="11.0"/>
+    <col customWidth="1" min="13" max="13" width="17.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -19831,45 +19832,45 @@
         <v>24</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>41</v>
@@ -20978,22 +20979,22 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>
@@ -22027,7 +22028,7 @@
         <v>54</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>
@@ -23058,10 +23059,10 @@
         <v>56</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>
@@ -24092,10 +24093,10 @@
         <v>57</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
RDBMS based persisetence for forms. Main features added
</commit_message>
<xml_diff>
--- a/src/main/resources/fm/spec/form/form2.xlsx
+++ b/src/main/resources/fm/spec/form/form2.xlsx
@@ -7,7 +7,7 @@
     <sheet state="visible" name="references" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="specialInstructions" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="fields" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="tables" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="childForms" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="fromToPairs" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="mutuallyExclusivePairs" sheetId="7" r:id="rId9"/>
     <sheet state="visible" name="mutuallyInclusivePairs" sheetId="8" r:id="rId10"/>
@@ -17,25 +17,19 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataSignature="AMtx7mj//Yg9YqpuJdwISlIG/Zcmkz6NWQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataSignature="AMtx7mgXXpdiFUbj4M27iFWRDC60uDOGzQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
-  <si>
-    <t>Sl No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Feature</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Reference</t>
+    <t>Sl No</t>
   </si>
   <si>
     <t>True/False</t>
@@ -44,13 +38,19 @@
     <t>Description</t>
   </si>
   <si>
-    <t>references to otherdocuments ofrelevance to this form</t>
+    <t>Note</t>
   </si>
   <si>
     <t>userIdFieldName</t>
   </si>
   <si>
+    <t>Reference</t>
+  </si>
+  <si>
     <t>All notes,including Q&amp;A about this form</t>
+  </si>
+  <si>
+    <t>references to otherdocuments ofrelevance to this form</t>
   </si>
   <si>
     <t>getAllowed</t>
@@ -98,13 +98,28 @@
     <t>pistSubmitProcessor</t>
   </si>
   <si>
-    <t>Field Name</t>
-  </si>
-  <si>
     <t>tableName</t>
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>Form Name</t>
+  </si>
+  <si>
+    <t>Min Rows</t>
+  </si>
+  <si>
+    <t>Max Rows</t>
+  </si>
+  <si>
+    <t>Link Fields From Parent</t>
+  </si>
+  <si>
+    <t>LInk Fields From Child</t>
+  </si>
+  <si>
+    <t>Field Name</t>
   </si>
   <si>
     <t>Place Holder</t>
@@ -134,16 +149,22 @@
     <t>value List Name</t>
   </si>
   <si>
-    <t>Form Name</t>
+    <t>Value List Key Field</t>
   </si>
   <si>
-    <t>Min Rows</t>
+    <t>dbColumnName</t>
   </si>
   <si>
-    <t>Max Rows</t>
+    <t>parentFieldName</t>
   </si>
   <si>
-    <t>Value List Key Field</t>
+    <t>customerId</t>
+  </si>
+  <si>
+    <t>Customer Id</t>
+  </si>
+  <si>
+    <t>customer_id</t>
   </si>
   <si>
     <t>productId</t>
@@ -159,6 +180,9 @@
   </si>
   <si>
     <t>textId</t>
+  </si>
+  <si>
+    <t>product_id</t>
   </si>
   <si>
     <t>quantity</t>
@@ -212,10 +236,10 @@
     </font>
     <font>
       <color rgb="FF00FF00"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF00FF00"/>
-      <name val="Arial"/>
     </font>
     <font/>
     <font>
@@ -277,14 +301,14 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -349,11 +373,11 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -376,7 +400,7 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -5778,11 +5802,11 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -5805,7 +5829,7 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -11208,14 +11232,14 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -11236,7 +11260,7 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -19809,7 +19833,12 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
@@ -19825,124 +19854,139 @@
     <col customWidth="1" min="10" max="10" width="9.14"/>
     <col customWidth="1" min="11" max="11" width="11.0"/>
     <col customWidth="1" min="13" max="13" width="17.14"/>
+    <col customWidth="1" min="14" max="14" width="17.57"/>
+    <col customWidth="1" min="15" max="15" width="18.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="D2" s="11"/>
       <c r="E2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="10" t="b">
+      <c r="H2" s="11" t="b">
         <v>1</v>
       </c>
       <c r="I2" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="10" t="b">
-        <v>0</v>
+      <c r="N2" s="10" t="s">
+        <v>46</v>
       </c>
-      <c r="K2" s="10" t="b">
+      <c r="O2" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="H3" s="10" t="b">
+      <c r="I3" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="10" t="b">
+      <c r="J3" s="11" t="b">
         <v>0</v>
       </c>
       <c r="K3" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
+      <c r="N3" s="10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="11" t="s">
-        <v>48</v>
+      <c r="A4" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>48</v>
+      <c r="E4" s="12" t="s">
+        <v>55</v>
       </c>
+      <c r="F4" s="11"/>
       <c r="H4" s="11" t="b">
         <v>1</v>
       </c>
@@ -19952,14 +19996,48 @@
       <c r="J4" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="K4" s="11" t="b">
+      <c r="K4" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="L4" s="11" t="s">
-        <v>51</v>
+      <c r="N4" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -20955,6 +21033,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -20979,22 +21058,28 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>38</v>
+        <v>28</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>
@@ -22019,16 +22104,16 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>
@@ -23053,16 +23138,16 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>
@@ -24087,16 +24172,16 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>
@@ -25120,10 +25205,10 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1"/>

</xml_diff>